<commit_message>
Merging of suites and updation of code
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/BulkOrders/BulkOrdersTestData.xlsx
+++ b/binaries/FCfiles/BulkOrders/BulkOrdersTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY\git\qualitesoft\binaries\FCfiles\BulkOrders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821F076A-01FC-4032-A608-1B379CC8E0C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF76DFC-55FF-4E2D-81E4-F3A933A31AFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F04869E1-D7A4-4938-9FF4-38A5495F3B22}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>FileName</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>BulkOrderUploadTemplate-AutoBook.xlsm</t>
+  </si>
+  <si>
+    <t>Carrier</t>
+  </si>
+  <si>
+    <t>Echo,Team Worldwide</t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD5EE64-FBAC-42F1-B944-30E4CC42AB9D}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +452,7 @@
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +471,11 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -482,8 +491,11 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Recording flat and existing scripts update
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/BulkOrders/BulkOrdersTestData.xlsx
+++ b/binaries/FCfiles/BulkOrders/BulkOrdersTestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY\git\qualitesoft\binaries\FCfiles\BulkOrders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF76DFC-55FF-4E2D-81E4-F3A933A31AFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D92F6D-45F0-43AB-915A-BE0A2C9FAE37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F04869E1-D7A4-4938-9FF4-38A5495F3B22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ContactInfo" sheetId="2" r:id="rId2"/>
+    <sheet name="Input" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>FileName</t>
   </si>
@@ -86,6 +87,9 @@
   </si>
   <si>
     <t>Echo,Team Worldwide</t>
+  </si>
+  <si>
+    <t>UPS</t>
   </si>
 </sst>
 </file>
@@ -109,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -117,12 +121,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +460,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,4 +579,29 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A1EBBB4-C4C5-4559-819C-6668569D706A}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>